<commit_message>
MOD: Se corrigio, que los datos Gtfs estaban separados mediante: punto y com (;), cuando la forma correcta es separarlos mediane comas (,). Se modifico el nombre del ejecutable.
</commit_message>
<xml_diff>
--- a/dist/Informacion.xlsx
+++ b/dist/Informacion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yagoramos\Desktop\BETA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yagoramos\Desktop\XlsxToGtfs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE55A70-F2A3-4B2B-9BD5-BF0FEA98BBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4709BF18-6731-4E02-AB0D-BB8FB9B23DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="811" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>